<commit_message>
Added Run for 90 days
</commit_message>
<xml_diff>
--- a/linearization_heuristic_dyn_models/linearization_heuristic_results_90_days.xlsx
+++ b/linearization_heuristic_dyn_models/linearization_heuristic_results_90_days.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,20 +462,30 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>lockdown_freq</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>reward</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>test_freq</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>testing</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>tests</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>xi</t>
         </is>
@@ -486,13 +496,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>22089.56346396808</v>
+        <v>1549.820285967816</v>
       </c>
       <c r="C2" t="n">
         <v>0.5</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>43844049464.29655</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -503,18 +513,24 @@
         <v>2000</v>
       </c>
       <c r="G2" t="n">
-        <v>-2332529839.07643</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>40250755195.01114</v>
       </c>
       <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
         <v>0</v>
       </c>
-      <c r="J2" t="n">
-        <v>0</v>
+      <c r="L2" t="n">
+        <v>2231941.8</v>
       </c>
     </row>
     <row r="3">
@@ -522,35 +538,41 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>22444.79953830915</v>
+        <v>1577.388424166159</v>
       </c>
       <c r="C3" t="n">
         <v>0.5</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>43845881124.38062</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>linearization_heuristic_Prop_Bouncing</t>
+          <t>linearization_heuristic</t>
         </is>
       </c>
       <c r="F3" t="n">
         <v>2000</v>
       </c>
       <c r="G3" t="n">
-        <v>-3104218115.362121</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
+        <v>14</v>
+      </c>
+      <c r="H3" t="n">
+        <v>40185246591.51936</v>
       </c>
       <c r="I3" t="n">
+        <v>7</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
         <v>0</v>
       </c>
-      <c r="J3" t="n">
-        <v>0</v>
+      <c r="L3" t="n">
+        <v>2231941.8</v>
       </c>
     </row>
     <row r="4">
@@ -558,35 +580,41 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>23786.41279629565</v>
+        <v>1549.799349952191</v>
       </c>
       <c r="C4" t="n">
         <v>0.5</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>43844049464.32219</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>linearization_heuristic</t>
+          <t>linearization_heuristic_Prop_Bouncing</t>
         </is>
       </c>
       <c r="F4" t="n">
         <v>2000</v>
       </c>
       <c r="G4" t="n">
-        <v>-2373274113.218047</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>40250806151.80891</v>
       </c>
       <c r="I4" t="n">
-        <v>30000</v>
-      </c>
-      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
         <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2231941.8</v>
       </c>
     </row>
     <row r="5">
@@ -594,13 +622,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>24161.1029046647</v>
+        <v>1577.369719139921</v>
       </c>
       <c r="C5" t="n">
         <v>0.5</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>43845881124.41301</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -611,18 +639,24 @@
         <v>2000</v>
       </c>
       <c r="G5" t="n">
-        <v>-3180384352.007998</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
+        <v>14</v>
+      </c>
+      <c r="H5" t="n">
+        <v>40185292430.46282</v>
       </c>
       <c r="I5" t="n">
-        <v>30000</v>
-      </c>
-      <c r="J5" t="n">
+        <v>7</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
         <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>2231941.8</v>
       </c>
     </row>
     <row r="6">
@@ -630,13 +664,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>24066.91794378401</v>
+        <v>1420.550188517038</v>
       </c>
       <c r="C6" t="n">
         <v>0.5</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>43986747680.24268</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -647,18 +681,24 @@
         <v>2000</v>
       </c>
       <c r="G6" t="n">
-        <v>-29762704211.95647</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>40703357020.42834</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1115970.9</v>
+        <v>1</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>30000</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2231941.8</v>
       </c>
     </row>
     <row r="7">
@@ -666,35 +706,41 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>24357.23370853326</v>
+        <v>1386.685491618477</v>
       </c>
       <c r="C7" t="n">
         <v>0.5</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>43973311978.57693</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>linearization_heuristic_Prop_Bouncing</t>
+          <t>linearization_heuristic</t>
         </is>
       </c>
       <c r="F7" t="n">
         <v>2000</v>
       </c>
       <c r="G7" t="n">
-        <v>-30640596520.94985</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
+        <v>14</v>
+      </c>
+      <c r="H7" t="n">
+        <v>40771049891.36427</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1115970.9</v>
+        <v>7</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>30000</v>
+      </c>
+      <c r="L7" t="n">
+        <v>2231941.8</v>
       </c>
     </row>
     <row r="8">
@@ -702,35 +748,41 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>23440.34122279853</v>
+        <v>1420.530868342983</v>
       </c>
       <c r="C8" t="n">
         <v>0.5</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>43986747680.24716</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>linearization_heuristic</t>
+          <t>linearization_heuristic_Prop_Bouncing</t>
         </is>
       </c>
       <c r="F8" t="n">
         <v>2000</v>
       </c>
       <c r="G8" t="n">
-        <v>-29006713587.66103</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>40703404012.3964</v>
       </c>
       <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
         <v>30000</v>
       </c>
-      <c r="J8" t="n">
-        <v>1115970.9</v>
+      <c r="L8" t="n">
+        <v>2231941.8</v>
       </c>
     </row>
     <row r="9">
@@ -738,13 +790,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>23724.10495496288</v>
+        <v>1386.669162326891</v>
       </c>
       <c r="C9" t="n">
         <v>0.5</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>43973311978.57693</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -755,18 +807,24 @@
         <v>2000</v>
       </c>
       <c r="G9" t="n">
-        <v>-29863687044.67785</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
+        <v>14</v>
+      </c>
+      <c r="H9" t="n">
+        <v>40771089914.89458</v>
       </c>
       <c r="I9" t="n">
+        <v>7</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
         <v>30000</v>
       </c>
-      <c r="J9" t="n">
-        <v>1115970.9</v>
+      <c r="L9" t="n">
+        <v>2231941.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added prints and explicit upper and lower bounds
</commit_message>
<xml_diff>
--- a/linearization_heuristic_dyn_models/linearization_heuristic_results_90_days.xlsx
+++ b/linearization_heuristic_dyn_models/linearization_heuristic_results_90_days.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,40 +452,45 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>eta</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>heuristic</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>icus</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>lockdown_freq</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>reward</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>test_freq</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>testing</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>tests</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>xi</t>
         </is>
@@ -496,41 +501,44 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>15919.79628449737</v>
+        <v>6.516444184994427</v>
       </c>
       <c r="C2" t="n">
         <v>0.5</v>
       </c>
       <c r="D2" t="n">
-        <v>13460015756.93711</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>3000</v>
+        <v>47272913542.61837</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="H2" t="n">
-        <v>-3852569451.521755</v>
+        <v>14</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>30000</v>
+        <v>40266439789.21677</v>
+      </c>
+      <c r="J2" t="n">
+        <v>7</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
       </c>
       <c r="L2" t="n">
-        <v>1000000</v>
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -538,41 +546,674 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>14226.1445856733</v>
+        <v>13.36631033395112</v>
       </c>
       <c r="C3" t="n">
         <v>0.5</v>
       </c>
       <c r="D3" t="n">
-        <v>13463415948.93342</v>
-      </c>
-      <c r="E3" t="inlineStr">
+        <v>60722901893.19477</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I3" t="n">
+        <v>50783118135.74285</v>
+      </c>
+      <c r="J3" t="n">
+        <v>7</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>6.515772677122709</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>47272913542.56073</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>40266439789.15913</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>13.36630322328767</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>60722901893.19476</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>50783118135.74284</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6.515709159910391</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>47272914048.2946</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>linearization_heuristic_Prop_Bouncing</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>3000</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>-1677804720.363207</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>linearization_heuristic</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>30000</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1000000</v>
+      <c r="G6" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H6" t="n">
+        <v>14</v>
+      </c>
+      <c r="I6" t="n">
+        <v>40266475658.14051</v>
+      </c>
+      <c r="J6" t="n">
+        <v>7</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>13.36624075229476</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>60722903030.43298</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_Prop_Bouncing</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>14</v>
+      </c>
+      <c r="I7" t="n">
+        <v>50783180916.52731</v>
+      </c>
+      <c r="J7" t="n">
+        <v>7</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>6.515709159910391</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>47272914048.23696</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_Prop_Bouncing</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>40266475658.08288</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>13.36624075229476</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>60722903030.43297</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_Prop_Bouncing</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>50783180916.52731</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>6.047501766411505</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>45984273238.28678</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H10" t="n">
+        <v>14</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-27904181031.53094</v>
+      </c>
+      <c r="J10" t="n">
+        <v>7</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>11159709000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>7.492154812950346</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>55979743228.85105</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H11" t="n">
+        <v>14</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-35482035577.2624</v>
+      </c>
+      <c r="J11" t="n">
+        <v>7</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>11159709000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>5.829154524567893</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D12" t="n">
+        <v>45260708538.65807</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-25921458881.12601</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>11159709000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>7.520932475781873</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>56200851177.3633</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-35579667356.82008</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>11159709000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>6.047486504859598</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>45984273680.48701</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_Prop_Bouncing</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H14" t="n">
+        <v>14</v>
+      </c>
+      <c r="I14" t="n">
+        <v>-27903979991.77816</v>
+      </c>
+      <c r="J14" t="n">
+        <v>7</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>11159709000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>7.49213530074887</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D15" t="n">
+        <v>55979743928.64222</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_Prop_Bouncing</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H15" t="n">
+        <v>14</v>
+      </c>
+      <c r="I15" t="n">
+        <v>-35481773689.28291</v>
+      </c>
+      <c r="J15" t="n">
+        <v>7</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>11159709000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>5.829140046103282</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D16" t="n">
+        <v>45260708950.42406</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_Prop_Bouncing</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>-25921268762.93503</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>11159709000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>7.520912947294536</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D17" t="n">
+        <v>56200851881.23368</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_Prop_Bouncing</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" t="n">
+        <v>-35579405521.63052</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>linearization_heuristic</t>
+        </is>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>11159709000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added runs for one group Lin Heur
</commit_message>
<xml_diff>
--- a/linearization_heuristic_dyn_models/linearization_heuristic_results_90_days.xlsx
+++ b/linearization_heuristic_dyn_models/linearization_heuristic_results_90_days.xlsx
@@ -501,13 +501,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.058298367644753</v>
+        <v>1.077172790289468</v>
       </c>
       <c r="C2" t="n">
         <v>0.5</v>
       </c>
       <c r="D2" t="n">
-        <v>46317314548.46852</v>
+        <v>46247219530.28053</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -524,7 +524,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>42825582311.74051</v>
+        <v>42693213333.75719</v>
       </c>
       <c r="J2" t="n">
         <v>1</v>
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -546,13 +546,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.361992657362816</v>
+        <v>1.800815659480598</v>
       </c>
       <c r="C3" t="n">
         <v>0.5</v>
       </c>
       <c r="D3" t="n">
-        <v>52792010116.85809</v>
+        <v>53502294527.56234</v>
       </c>
       <c r="E3" t="n">
         <v>0.1</v>
@@ -569,7 +569,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>48298273933.09697</v>
+        <v>47560712944.47166</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -591,13 +591,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.108517102734018</v>
+        <v>1.130337585097727</v>
       </c>
       <c r="C4" t="n">
         <v>0.5</v>
       </c>
       <c r="D4" t="n">
-        <v>46441108725.47605</v>
+        <v>46385782023.66711</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -614,7 +614,7 @@
         <v>14</v>
       </c>
       <c r="I4" t="n">
-        <v>42783685619.74567</v>
+        <v>42656364777.13512</v>
       </c>
       <c r="J4" t="n">
         <v>7</v>
@@ -625,7 +625,7 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -636,13 +636,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.424606802960026</v>
+        <v>1.794814984367979</v>
       </c>
       <c r="C5" t="n">
         <v>0.5</v>
       </c>
       <c r="D5" t="n">
-        <v>52917919417.56814</v>
+        <v>53426790567.65892</v>
       </c>
       <c r="E5" t="n">
         <v>0.1</v>
@@ -659,7 +659,7 @@
         <v>14</v>
       </c>
       <c r="I5" t="n">
-        <v>48217595151.14416</v>
+        <v>47505007513.38911</v>
       </c>
       <c r="J5" t="n">
         <v>7</v>
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -681,13 +681,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.058298367644753</v>
+        <v>1.077172790289468</v>
       </c>
       <c r="C6" t="n">
         <v>0.5</v>
       </c>
       <c r="D6" t="n">
-        <v>46317314548.46852</v>
+        <v>46247219530.28053</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -704,7 +704,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>42825582311.74051</v>
+        <v>42693213333.75719</v>
       </c>
       <c r="J6" t="n">
         <v>1</v>
@@ -715,7 +715,7 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -726,13 +726,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.361992657362816</v>
+        <v>1.800815659480598</v>
       </c>
       <c r="C7" t="n">
         <v>0.5</v>
       </c>
       <c r="D7" t="n">
-        <v>52792010116.85809</v>
+        <v>53502294527.56234</v>
       </c>
       <c r="E7" t="n">
         <v>0.1</v>
@@ -749,7 +749,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>48298273933.09697</v>
+        <v>47560712944.47166</v>
       </c>
       <c r="J7" t="n">
         <v>1</v>
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -771,13 +771,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1.108517102734018</v>
+        <v>1.130337585097727</v>
       </c>
       <c r="C8" t="n">
         <v>0.5</v>
       </c>
       <c r="D8" t="n">
-        <v>46441108725.47605</v>
+        <v>46385782023.66711</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -794,7 +794,7 @@
         <v>14</v>
       </c>
       <c r="I8" t="n">
-        <v>42783685619.74567</v>
+        <v>42656364777.13512</v>
       </c>
       <c r="J8" t="n">
         <v>7</v>
@@ -805,7 +805,7 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
@@ -816,13 +816,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1.424606802960026</v>
+        <v>1.794814984367979</v>
       </c>
       <c r="C9" t="n">
         <v>0.5</v>
       </c>
       <c r="D9" t="n">
-        <v>52917919417.56814</v>
+        <v>53426790567.65892</v>
       </c>
       <c r="E9" t="n">
         <v>0.1</v>
@@ -839,7 +839,7 @@
         <v>14</v>
       </c>
       <c r="I9" t="n">
-        <v>48217595151.14416</v>
+        <v>47505007513.38911</v>
       </c>
       <c r="J9" t="n">
         <v>7</v>
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="L9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
@@ -861,13 +861,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.6034344150864958</v>
+        <v>0.6393717843845849</v>
       </c>
       <c r="C10" t="n">
         <v>0.5</v>
       </c>
       <c r="D10" t="n">
-        <v>43147341045.45089</v>
+        <v>43196586691.04309</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -884,7 +884,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>34422226983.28634</v>
+        <v>33951850879.80246</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -895,7 +895,7 @@
         </is>
       </c>
       <c r="L10" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
         <v>11159709000</v>
@@ -906,13 +906,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.6271818492969048</v>
+        <v>0.7552459685402271</v>
       </c>
       <c r="C11" t="n">
         <v>0.5</v>
       </c>
       <c r="D11" t="n">
-        <v>48569441960.47471</v>
+        <v>48153337817.38026</v>
       </c>
       <c r="E11" t="n">
         <v>0.1</v>
@@ -929,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>39500961548.9781</v>
+        <v>37233166452.01514</v>
       </c>
       <c r="J11" t="n">
         <v>1</v>
@@ -940,7 +940,7 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
         <v>11159709000</v>
@@ -951,13 +951,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.6021885435055344</v>
+        <v>0.6164307654473636</v>
       </c>
       <c r="C12" t="n">
         <v>0.5</v>
       </c>
       <c r="D12" t="n">
-        <v>42846866826.35518</v>
+        <v>42578077213.51637</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -974,7 +974,7 @@
         <v>14</v>
       </c>
       <c r="I12" t="n">
-        <v>34139766936.69876</v>
+        <v>33665047718.53025</v>
       </c>
       <c r="J12" t="n">
         <v>7</v>
@@ -985,7 +985,7 @@
         </is>
       </c>
       <c r="L12" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
         <v>11159709000</v>
@@ -996,13 +996,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.6448691365100838</v>
+        <v>0.7574598594689712</v>
       </c>
       <c r="C13" t="n">
         <v>0.5</v>
       </c>
       <c r="D13" t="n">
-        <v>48547780458.98592</v>
+        <v>47985365362.29326</v>
       </c>
       <c r="E13" t="n">
         <v>0.1</v>
@@ -1019,7 +1019,7 @@
         <v>14</v>
       </c>
       <c r="I13" t="n">
-        <v>39223557924.52286</v>
+        <v>37033183143.0697</v>
       </c>
       <c r="J13" t="n">
         <v>7</v>
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
         <v>11159709000</v>
@@ -1041,13 +1041,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.6034344150864958</v>
+        <v>0.6393717843845849</v>
       </c>
       <c r="C14" t="n">
         <v>0.5</v>
       </c>
       <c r="D14" t="n">
-        <v>43147341045.45089</v>
+        <v>43196586691.04309</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -1064,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>34422226983.28634</v>
+        <v>33951850879.80246</v>
       </c>
       <c r="J14" t="n">
         <v>1</v>
@@ -1075,7 +1075,7 @@
         </is>
       </c>
       <c r="L14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M14" t="n">
         <v>11159709000</v>
@@ -1086,13 +1086,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.6271818492969047</v>
+        <v>0.7552459685402206</v>
       </c>
       <c r="C15" t="n">
         <v>0.5</v>
       </c>
       <c r="D15" t="n">
-        <v>48569441960.47471</v>
+        <v>48153337817.38026</v>
       </c>
       <c r="E15" t="n">
         <v>0.1</v>
@@ -1109,7 +1109,7 @@
         <v>1</v>
       </c>
       <c r="I15" t="n">
-        <v>39500961548.9781</v>
+        <v>37233166452.01523</v>
       </c>
       <c r="J15" t="n">
         <v>1</v>
@@ -1120,7 +1120,7 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M15" t="n">
         <v>11159709000</v>
@@ -1131,13 +1131,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.6021885435055344</v>
+        <v>0.6164307654473636</v>
       </c>
       <c r="C16" t="n">
         <v>0.5</v>
       </c>
       <c r="D16" t="n">
-        <v>42846866826.35518</v>
+        <v>42578077213.51637</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1154,7 +1154,7 @@
         <v>14</v>
       </c>
       <c r="I16" t="n">
-        <v>34139766936.69876</v>
+        <v>33665047718.53025</v>
       </c>
       <c r="J16" t="n">
         <v>7</v>
@@ -1165,7 +1165,7 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M16" t="n">
         <v>11159709000</v>
@@ -1176,13 +1176,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.6448691365100838</v>
+        <v>0.757459859468971</v>
       </c>
       <c r="C17" t="n">
         <v>0.5</v>
       </c>
       <c r="D17" t="n">
-        <v>48547780458.98592</v>
+        <v>47985365362.29326</v>
       </c>
       <c r="E17" t="n">
         <v>0.1</v>
@@ -1199,7 +1199,7 @@
         <v>14</v>
       </c>
       <c r="I17" t="n">
-        <v>39223557924.52286</v>
+        <v>37033183143.0697</v>
       </c>
       <c r="J17" t="n">
         <v>7</v>
@@ -1210,7 +1210,7 @@
         </is>
       </c>
       <c r="L17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M17" t="n">
         <v>11159709000</v>

</xml_diff>